<commit_message>
Feat(company job): Update example job upload form.
</commit_message>
<xml_diff>
--- a/OpenHouse/static/file/oh_job_upload.xlsx
+++ b/OpenHouse/static/file/oh_job_upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsun/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony2\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75167157-CF76-AC47-BB99-8765FF74295F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DB27C9-3A85-49AA-8745-C57F956BCA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -33,16 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>備註(260字內)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>職缺內容(英文)(260字內)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>職缺名稱(英文)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -76,6 +72,397 @@
   </si>
   <si>
     <t>職缺內容(必填，260字內)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>學歷條件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(260</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>字內</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>福利制度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(260</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>字內</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>薪資待遇</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(260</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>字內</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>職缺內容</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>英文</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)(Up to 780 English characters)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>學歷條件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>英文</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)(Up to 780 English characters)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>薪資待遇</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>英文</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)(Up to 780 English characters)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>福利制度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>英文</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)(Up to 780 English characters)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>休假制度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>英文</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)(Up to 780 English characters)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>休假制度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(260</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>字內</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -83,7 +470,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -111,6 +498,34 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,13 +547,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -357,54 +774,87 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="38.5703125" customWidth="1"/>
+    <col min="13" max="13" width="39.7109375" customWidth="1"/>
+    <col min="14" max="14" width="39" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" customWidth="1"/>
+    <col min="16" max="16" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:17" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -416,14 +866,22 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -434,7 +892,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -445,7 +903,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -456,7 +914,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -467,7 +925,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -478,7 +936,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -489,7 +947,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -500,7 +958,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -511,7 +969,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -522,7 +980,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -533,7 +991,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -544,7 +1002,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -555,7 +1013,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -566,7 +1024,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>